<commit_message>
Atualização da inserção de veículos
</commit_message>
<xml_diff>
--- a/banco-de-dados/Modelagem/TESTEDEMESA_MODELAGEM.xlsx
+++ b/banco-de-dados/Modelagem/TESTEDEMESA_MODELAGEM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12970" windowHeight="6370" tabRatio="816" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12970" windowHeight="6370" tabRatio="816" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Veiculo" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="174">
   <si>
     <t>Marca_veiculo</t>
   </si>
@@ -576,12 +576,12 @@
   <numFmts count="8">
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="######0"/>
-    <numFmt numFmtId="172" formatCode="0000####"/>
-    <numFmt numFmtId="173" formatCode="0000#"/>
-    <numFmt numFmtId="174" formatCode="00000#"/>
-    <numFmt numFmtId="175" formatCode="000000#"/>
-    <numFmt numFmtId="176" formatCode="000#"/>
-    <numFmt numFmtId="177" formatCode="00#"/>
+    <numFmt numFmtId="166" formatCode="0000####"/>
+    <numFmt numFmtId="167" formatCode="0000#"/>
+    <numFmt numFmtId="168" formatCode="00000#"/>
+    <numFmt numFmtId="169" formatCode="000000#"/>
+    <numFmt numFmtId="170" formatCode="000#"/>
+    <numFmt numFmtId="171" formatCode="00#"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -662,24 +662,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="174" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="175" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -962,10 +962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U134"/>
+  <dimension ref="A1:U131"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G1"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1111,7 +1111,7 @@
         <v>9</v>
       </c>
       <c r="R2" s="9">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="S2" t="s">
         <v>170</v>
@@ -1176,7 +1176,7 @@
         <v>16</v>
       </c>
       <c r="R3" s="9">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="S3" t="s">
         <v>17</v>
@@ -1241,7 +1241,7 @@
         <v>16</v>
       </c>
       <c r="R4" s="9">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="S4" t="s">
         <v>22</v>
@@ -1306,7 +1306,7 @@
         <v>16</v>
       </c>
       <c r="R5" s="9">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="S5" t="s">
         <v>33</v>
@@ -1371,7 +1371,7 @@
         <v>16</v>
       </c>
       <c r="R6" s="9">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="S6" t="s">
         <v>38</v>
@@ -1436,7 +1436,7 @@
         <v>16</v>
       </c>
       <c r="R7" s="9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S7" t="s">
         <v>17</v>
@@ -1501,7 +1501,7 @@
         <v>16</v>
       </c>
       <c r="R8" s="9">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="S8" t="s">
         <v>47</v>
@@ -1566,7 +1566,7 @@
         <v>16</v>
       </c>
       <c r="R9" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S9" t="s">
         <v>52</v>
@@ -1631,7 +1631,7 @@
         <v>16</v>
       </c>
       <c r="R10" s="9">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="S10" t="s">
         <v>52</v>
@@ -1696,7 +1696,7 @@
         <v>16</v>
       </c>
       <c r="R11" s="9">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="S11" t="s">
         <v>56</v>
@@ -1761,7 +1761,7 @@
         <v>9</v>
       </c>
       <c r="R12" s="9">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="S12" t="s">
         <v>59</v>
@@ -1826,7 +1826,7 @@
         <v>16</v>
       </c>
       <c r="R13" s="9">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="S13" t="s">
         <v>65</v>
@@ -1891,7 +1891,7 @@
         <v>9</v>
       </c>
       <c r="R14" s="9">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="S14" t="s">
         <v>68</v>
@@ -1956,7 +1956,7 @@
         <v>73</v>
       </c>
       <c r="R15" s="9">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="S15" t="s">
         <v>75</v>
@@ -2021,7 +2021,7 @@
         <v>16</v>
       </c>
       <c r="R16" s="9">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="S16" t="s">
         <v>90</v>
@@ -2086,7 +2086,7 @@
         <v>16</v>
       </c>
       <c r="R17" s="9">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="S17" t="s">
         <v>93</v>
@@ -2151,7 +2151,7 @@
         <v>16</v>
       </c>
       <c r="R18" s="9">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="S18" t="s">
         <v>99</v>
@@ -2216,7 +2216,7 @@
         <v>16</v>
       </c>
       <c r="R19" s="9">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="S19" t="s">
         <v>105</v>
@@ -2230,31 +2230,31 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="15">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="D20" s="11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="F20" s="11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G20" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="H20" s="8">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I20" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="J20" s="16">
         <v>2</v>
@@ -2263,45 +2263,45 @@
         <v>103</v>
       </c>
       <c r="L20" s="6">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="M20">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="N20" s="9">
+        <v>3</v>
+      </c>
+      <c r="O20" t="s">
+        <v>31</v>
+      </c>
+      <c r="P20" s="18">
         <v>2</v>
       </c>
-      <c r="O20" t="s">
-        <v>30</v>
-      </c>
-      <c r="P20" s="18">
-        <v>1</v>
-      </c>
       <c r="Q20" t="s">
-        <v>16</v>
+        <v>115</v>
       </c>
       <c r="R20" s="9">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="S20" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="T20" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="U20" s="2">
-        <v>260000</v>
+        <v>240000</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D21" s="11">
         <v>7</v>
@@ -2316,57 +2316,57 @@
         <v>109</v>
       </c>
       <c r="H21" s="8">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I21" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="J21" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K21" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="L21" s="6">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="M21">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="N21" s="9">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O21" t="s">
-        <v>31</v>
+        <v>121</v>
       </c>
       <c r="P21" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q21" t="s">
-        <v>115</v>
+        <v>16</v>
       </c>
       <c r="R21" s="9">
         <v>20</v>
       </c>
       <c r="S21" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="T21" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="U21" s="2">
-        <v>240000</v>
+        <v>550000</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="D22" s="11">
         <v>7</v>
@@ -2381,28 +2381,28 @@
         <v>109</v>
       </c>
       <c r="H22" s="8">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I22" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="J22" s="16">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K22" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="L22" s="6">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="M22">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="N22" s="9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O22" t="s">
-        <v>121</v>
+        <v>31</v>
       </c>
       <c r="P22" s="18">
         <v>1</v>
@@ -2411,27 +2411,27 @@
         <v>16</v>
       </c>
       <c r="R22" s="9">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="S22" t="s">
         <v>122</v>
       </c>
       <c r="T22" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="U22" s="2">
-        <v>550000</v>
+        <v>790000</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="D23" s="11">
         <v>7</v>
@@ -2446,22 +2446,22 @@
         <v>109</v>
       </c>
       <c r="H23" s="8">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I23" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="J23" s="16">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K23" t="s">
-        <v>43</v>
+        <v>131</v>
       </c>
       <c r="L23" s="6">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="M23">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="N23" s="9">
         <v>3</v>
@@ -2476,27 +2476,27 @@
         <v>16</v>
       </c>
       <c r="R23" s="9">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="S23" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="T23" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="U23" s="2">
-        <v>790000</v>
+        <v>1250000</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" s="15">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="D24" s="11">
         <v>7</v>
@@ -2511,16 +2511,16 @@
         <v>109</v>
       </c>
       <c r="H24" s="8">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I24" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="J24" s="16">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K24" t="s">
-        <v>131</v>
+        <v>35</v>
       </c>
       <c r="L24" s="6">
         <v>2021</v>
@@ -2541,27 +2541,27 @@
         <v>16</v>
       </c>
       <c r="R24" s="9">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="S24" t="s">
         <v>132</v>
       </c>
       <c r="T24" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="U24" s="2">
-        <v>1250000</v>
+        <v>1180000</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D25" s="11">
         <v>7</v>
@@ -2576,22 +2576,22 @@
         <v>109</v>
       </c>
       <c r="H25" s="8">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I25" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="J25" s="16">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K25" t="s">
-        <v>35</v>
+        <v>103</v>
       </c>
       <c r="L25" s="6">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="M25">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="N25" s="9">
         <v>3</v>
@@ -2600,33 +2600,33 @@
         <v>31</v>
       </c>
       <c r="P25" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q25" t="s">
-        <v>16</v>
+        <v>115</v>
       </c>
       <c r="R25" s="9">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="S25" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="T25" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="U25" s="2">
-        <v>1180000</v>
+        <v>175000</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26" s="15">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D26" s="11">
         <v>7</v>
@@ -2641,22 +2641,22 @@
         <v>109</v>
       </c>
       <c r="H26" s="8">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I26" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="J26" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K26" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="L26" s="6">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="M26">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="N26" s="9">
         <v>3</v>
@@ -2665,51 +2665,51 @@
         <v>31</v>
       </c>
       <c r="P26" s="18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q26" t="s">
-        <v>115</v>
+        <v>9</v>
       </c>
       <c r="R26" s="9">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="S26" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="T26" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="U26" s="2">
-        <v>175000</v>
+        <v>790000</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27" s="15">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="D27" s="11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E27" t="s">
-        <v>109</v>
+        <v>150</v>
       </c>
       <c r="F27" s="11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G27" t="s">
-        <v>109</v>
+        <v>150</v>
       </c>
       <c r="H27" s="8">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I27" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="J27" s="16">
         <v>5</v>
@@ -2718,75 +2718,75 @@
         <v>35</v>
       </c>
       <c r="L27" s="6">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="M27">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="N27" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O27" t="s">
-        <v>31</v>
+        <v>155</v>
       </c>
       <c r="P27" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q27" t="s">
-        <v>115</v>
+        <v>16</v>
       </c>
       <c r="R27" s="9">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="S27" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="T27" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="U27" s="2">
-        <v>175000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" s="15">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="D28" s="11">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E28" t="s">
-        <v>109</v>
+        <v>157</v>
       </c>
       <c r="F28" s="11">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G28" t="s">
-        <v>109</v>
+        <v>157</v>
       </c>
       <c r="H28" s="8">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I28" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="J28" s="16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K28" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="L28" s="6">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="M28">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="N28" s="9">
         <v>3</v>
@@ -2795,225 +2795,57 @@
         <v>31</v>
       </c>
       <c r="P28" s="18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q28" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="R28" s="9">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="S28" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="T28" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="U28" s="2">
-        <v>790000</v>
+        <v>1350000</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A29" s="15">
-        <v>25</v>
-      </c>
-      <c r="B29" t="s">
-        <v>149</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D29" s="11">
-        <v>8</v>
-      </c>
-      <c r="E29" t="s">
-        <v>150</v>
-      </c>
-      <c r="F29" s="11">
-        <v>8</v>
-      </c>
-      <c r="G29" t="s">
-        <v>150</v>
-      </c>
-      <c r="H29" s="8">
-        <v>25</v>
-      </c>
-      <c r="I29" t="s">
-        <v>151</v>
-      </c>
-      <c r="J29" s="16">
-        <v>5</v>
-      </c>
-      <c r="K29" t="s">
-        <v>35</v>
-      </c>
-      <c r="L29" s="6">
-        <v>2021</v>
-      </c>
-      <c r="M29">
-        <v>2021</v>
-      </c>
-      <c r="N29" s="9">
-        <v>4</v>
-      </c>
-      <c r="O29" t="s">
-        <v>155</v>
-      </c>
-      <c r="P29" s="18">
-        <v>1</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>16</v>
-      </c>
-      <c r="R29" s="9">
-        <v>3</v>
-      </c>
-      <c r="S29" t="s">
-        <v>154</v>
-      </c>
-      <c r="T29" t="s">
-        <v>153</v>
-      </c>
-      <c r="U29" s="2">
-        <v>3000000</v>
-      </c>
+      <c r="A29" s="13"/>
+      <c r="D29" s="11"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="17"/>
+      <c r="N29" s="9"/>
+      <c r="P29" s="18"/>
+      <c r="R29" s="9"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A30" s="15">
-        <v>25</v>
-      </c>
-      <c r="B30" t="s">
-        <v>149</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D30" s="11">
-        <v>8</v>
-      </c>
-      <c r="E30" t="s">
-        <v>150</v>
-      </c>
-      <c r="F30" s="11">
-        <v>8</v>
-      </c>
-      <c r="G30" t="s">
-        <v>150</v>
-      </c>
-      <c r="H30" s="8">
-        <v>25</v>
-      </c>
-      <c r="I30" t="s">
-        <v>151</v>
-      </c>
-      <c r="J30" s="16">
-        <v>1</v>
-      </c>
-      <c r="K30" t="s">
-        <v>13</v>
-      </c>
-      <c r="L30" s="6">
-        <v>2021</v>
-      </c>
-      <c r="M30">
-        <v>2021</v>
-      </c>
-      <c r="N30" s="9">
-        <v>4</v>
-      </c>
-      <c r="O30" t="s">
-        <v>155</v>
-      </c>
-      <c r="P30" s="18">
-        <v>1</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>16</v>
-      </c>
-      <c r="R30" s="9">
-        <v>3</v>
-      </c>
-      <c r="S30" t="s">
-        <v>154</v>
-      </c>
-      <c r="T30" t="s">
-        <v>153</v>
-      </c>
-      <c r="U30" s="2">
-        <v>3000000</v>
-      </c>
+      <c r="A30" s="13"/>
+      <c r="D30" s="11"/>
+      <c r="H30" s="8"/>
+      <c r="J30" s="16"/>
+      <c r="N30" s="9"/>
+      <c r="P30" s="18"/>
+      <c r="R30" s="9"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A31" s="15">
-        <v>26</v>
-      </c>
-      <c r="B31" t="s">
-        <v>156</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D31" s="11">
-        <v>9</v>
-      </c>
-      <c r="E31" t="s">
-        <v>157</v>
-      </c>
-      <c r="F31" s="11">
-        <v>9</v>
-      </c>
-      <c r="G31" t="s">
-        <v>157</v>
-      </c>
-      <c r="H31" s="8">
-        <v>26</v>
-      </c>
-      <c r="I31" t="s">
-        <v>158</v>
-      </c>
-      <c r="J31" s="16">
-        <v>3</v>
-      </c>
-      <c r="K31" t="s">
-        <v>21</v>
-      </c>
-      <c r="L31" s="6">
-        <v>2020</v>
-      </c>
-      <c r="M31">
-        <v>2020</v>
-      </c>
-      <c r="N31" s="9">
-        <v>3</v>
-      </c>
-      <c r="O31" t="s">
-        <v>31</v>
-      </c>
-      <c r="P31" s="18">
-        <v>1</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>16</v>
-      </c>
-      <c r="R31" s="9">
-        <v>22</v>
-      </c>
-      <c r="S31" t="s">
-        <v>161</v>
-      </c>
-      <c r="T31" t="s">
-        <v>159</v>
-      </c>
-      <c r="U31" s="2">
-        <v>1350000</v>
-      </c>
+      <c r="A31" s="13"/>
+      <c r="D31" s="11"/>
+      <c r="H31" s="8"/>
+      <c r="J31" s="16"/>
+      <c r="N31" s="9"/>
+      <c r="P31" s="18"/>
+      <c r="R31" s="9"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32" s="13"/>
       <c r="D32" s="11"/>
       <c r="H32" s="8"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="17"/>
+      <c r="J32" s="16"/>
       <c r="N32" s="9"/>
       <c r="P32" s="18"/>
       <c r="R32" s="9"/>
@@ -3606,45 +3438,30 @@
     <row r="98" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A98" s="13"/>
       <c r="D98" s="11"/>
-      <c r="H98" s="8"/>
-      <c r="J98" s="16"/>
-      <c r="N98" s="9"/>
       <c r="P98" s="18"/>
-      <c r="R98" s="9"/>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A99" s="13"/>
-      <c r="D99" s="11"/>
-      <c r="H99" s="8"/>
-      <c r="J99" s="16"/>
-      <c r="N99" s="9"/>
       <c r="P99" s="18"/>
-      <c r="R99" s="9"/>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A100" s="13"/>
-      <c r="D100" s="11"/>
-      <c r="H100" s="8"/>
-      <c r="J100" s="16"/>
-      <c r="N100" s="9"/>
       <c r="P100" s="18"/>
-      <c r="R100" s="9"/>
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A101" s="13"/>
-      <c r="D101" s="11"/>
       <c r="P101" s="18"/>
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A102" s="13"/>
+      <c r="A102" s="14"/>
       <c r="P102" s="18"/>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A103" s="13"/>
+      <c r="A103" s="14"/>
       <c r="P103" s="18"/>
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A104" s="13"/>
+      <c r="A104" s="14"/>
       <c r="P104" s="18"/>
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.35">
@@ -3661,15 +3478,12 @@
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A108" s="14"/>
-      <c r="P108" s="18"/>
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A109" s="14"/>
-      <c r="P109" s="18"/>
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A110" s="14"/>
-      <c r="P110" s="18"/>
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A111" s="14"/>
@@ -3733,15 +3547,6 @@
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A131" s="14"/>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A132" s="14"/>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A133" s="14"/>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A134" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -4499,205 +4304,331 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>169</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="9">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="9">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="9">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="9">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="9">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+      <c r="C15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+      <c r="C16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="9">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+      <c r="C17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="9">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+      <c r="C18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+      <c r="C19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="9">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+      <c r="C20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="9">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+      <c r="C21" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="9">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+      <c r="C22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="9">
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="9">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="9">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>142</v>
+      </c>
+      <c r="C25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="9">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>147</v>
+      </c>
+      <c r="C26" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="9">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>154</v>
+      </c>
+      <c r="C27" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="9">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
         <v>161</v>
+      </c>
+      <c r="C28" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4705,7 +4636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>